<commit_message>
added PTFE properties to material data excel doc'
</commit_message>
<xml_diff>
--- a/Materials/Materialproperties.xlsx
+++ b/Materials/Materialproperties.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="87">
   <si>
     <t>Material Properties</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>-54 to 149 C</t>
-  </si>
-  <si>
-    <t>112-135 m/m-K</t>
   </si>
   <si>
     <t>19.4e-6 in/in-F</t>
@@ -288,6 +285,38 @@
   </si>
   <si>
     <t>PTFE (General)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86e-6 +/- 3e-6 </t>
+  </si>
+  <si>
+    <t>(1956 Kirby text)</t>
+  </si>
+  <si>
+    <t>112-135 e-6m/m-K</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CTE of Teflon PTFE (+25 to -190C)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -399,13 +428,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>206459</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>72174</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>228069</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -443,13 +472,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>54272</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>8345</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>66899</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -783,18 +812,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -808,38 +837,40 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>7</v>
+      <c r="C6" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="E6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -848,7 +879,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -856,43 +887,38 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
         <v>73</v>
       </c>
-      <c r="D12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="E13" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -900,41 +926,41 @@
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" t="s">
-        <v>68</v>
+      <c r="C15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>4</v>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="D16" t="s">
         <v>67</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
@@ -942,13 +968,13 @@
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
@@ -956,13 +982,13 @@
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18">
-        <v>0.33</v>
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -970,137 +996,137 @@
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="D19">
+        <v>0.33</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C21" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>2</v>
+      <c r="C22" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>65</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C25" s="4" t="s">
-        <v>41</v>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" ht="45" x14ac:dyDescent="0.25">
       <c r="C26" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C27" s="4" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C28" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>57</v>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
+        <v>62</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C29" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" t="s">
-        <v>47</v>
+    <row r="29" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
@@ -1108,13 +1134,13 @@
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="4" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
@@ -1122,44 +1148,41 @@
     </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="6">
-        <v>4.7</v>
+        <v>47</v>
+      </c>
+      <c r="D31" t="s">
+        <v>48</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C32" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="D32" s="6">
+        <v>4.7</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
-      <c r="I32" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="33" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C33" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
@@ -1168,46 +1191,49 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C34" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="6">
-        <v>11.6</v>
+        <v>52</v>
+      </c>
+      <c r="D34" t="s">
+        <v>53</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D35" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="D35" s="6">
+        <v>11.6</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
+      <c r="I35" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D36" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -1215,84 +1241,84 @@
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="6">
-        <v>7.9</v>
+        <v>59</v>
+      </c>
+      <c r="D37" t="s">
+        <v>60</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
+      </c>
+      <c r="D38" s="6">
+        <v>7.9</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
+    <row r="39" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C40" s="2" t="s">
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-    </row>
-    <row r="42" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C42" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D42" t="s">
-        <v>24</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
     </row>
     <row r="43" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C43" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D43" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
@@ -1300,13 +1326,13 @@
     </row>
     <row r="44" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C44" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D44" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
@@ -1314,13 +1340,13 @@
     </row>
     <row r="45" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C45" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
@@ -1328,13 +1354,13 @@
     </row>
     <row r="46" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C46" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D46" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
@@ -1342,53 +1368,53 @@
     </row>
     <row r="47" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C47" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D47" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E48" s="7"/>
+    <row r="48" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C48" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C49" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" t="s">
-        <v>13</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
+      <c r="C50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E51" s="10" t="s">
         <v>14</v>
@@ -1399,10 +1425,10 @@
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D52" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E52" s="10" t="s">
         <v>14</v>
@@ -1413,60 +1439,42 @@
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>17</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="D53" t="s">
+        <v>16</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
     </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+    </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="E32:H32"/>
-    <mergeCell ref="E33:H33"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="E40:H40"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="E43:H43"/>
-    <mergeCell ref="E44:H44"/>
-    <mergeCell ref="E41:H41"/>
-    <mergeCell ref="E45:H45"/>
-    <mergeCell ref="E46:H46"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="E53:H53"/>
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="E50:H50"/>
-    <mergeCell ref="E51:H51"/>
-    <mergeCell ref="E52:H52"/>
-    <mergeCell ref="E36:H36"/>
     <mergeCell ref="E37:H37"/>
     <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="E23:H23"/>
     <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E15:H15"/>
     <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="E20:H20"/>
     <mergeCell ref="E24:H24"/>
     <mergeCell ref="E25:H25"/>
     <mergeCell ref="E26:H26"/>
@@ -1474,23 +1482,55 @@
     <mergeCell ref="E28:H28"/>
     <mergeCell ref="E29:H29"/>
     <mergeCell ref="E30:H30"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="E46:H46"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="E54:H54"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="E50:H50"/>
+    <mergeCell ref="E51:H51"/>
+    <mergeCell ref="E52:H52"/>
+    <mergeCell ref="E53:H53"/>
+    <mergeCell ref="E41:H41"/>
+    <mergeCell ref="E43:H43"/>
+    <mergeCell ref="E44:H44"/>
+    <mergeCell ref="E45:H45"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="E42" r:id="rId2"/>
-    <hyperlink ref="E43" r:id="rId3"/>
-    <hyperlink ref="E44" r:id="rId4"/>
-    <hyperlink ref="E45" r:id="rId5"/>
-    <hyperlink ref="E46" r:id="rId6"/>
-    <hyperlink ref="E47" r:id="rId7"/>
-    <hyperlink ref="E13:H13" r:id="rId8" display="matweb"/>
-    <hyperlink ref="E12:H12" r:id="rId9" display="matweb"/>
-    <hyperlink ref="E15:H15" r:id="rId10" display="matweb"/>
-    <hyperlink ref="E17:H17" r:id="rId11" display="matweb"/>
-    <hyperlink ref="E19:H19" r:id="rId12" display="matweb"/>
-    <hyperlink ref="E14:H14" r:id="rId13" display="matweb"/>
-    <hyperlink ref="E16:H16" r:id="rId14" display="matweb"/>
-    <hyperlink ref="E18:H18" r:id="rId15" display="matweb"/>
+    <hyperlink ref="E7" r:id="rId1"/>
+    <hyperlink ref="E43" r:id="rId2"/>
+    <hyperlink ref="E44" r:id="rId3"/>
+    <hyperlink ref="E45" r:id="rId4"/>
+    <hyperlink ref="E46" r:id="rId5"/>
+    <hyperlink ref="E47" r:id="rId6"/>
+    <hyperlink ref="E48" r:id="rId7"/>
+    <hyperlink ref="E14:H14" r:id="rId8" display="matweb"/>
+    <hyperlink ref="E13:H13" r:id="rId9" display="matweb"/>
+    <hyperlink ref="E16:H16" r:id="rId10" display="matweb"/>
+    <hyperlink ref="E18:H18" r:id="rId11" display="matweb"/>
+    <hyperlink ref="E20:H20" r:id="rId12" display="matweb"/>
+    <hyperlink ref="E15:H15" r:id="rId13" display="matweb"/>
+    <hyperlink ref="E17:H17" r:id="rId14" display="matweb"/>
+    <hyperlink ref="E19:H19" r:id="rId15" display="matweb"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId16"/>

</xml_diff>

<commit_message>
Updated Material property sheet
</commit_message>
<xml_diff>
--- a/Materials/Materialproperties.xlsx
+++ b/Materials/Materialproperties.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexf\git\composite-propellant-tank\Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\khensu\Home06\afarias\Desktop\git\composite-propellant-tank\Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18260" windowHeight="9050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18255" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="89">
   <si>
     <t>Material Properties</t>
   </si>
@@ -273,15 +273,6 @@
   </si>
   <si>
     <t>matweb</t>
-  </si>
-  <si>
-    <t>kx: in-plane thermal conductivity</t>
-  </si>
-  <si>
-    <t>ky: through thickness thermal conductivity</t>
-  </si>
-  <si>
-    <t>Source: Anisotrpic Thermal Property Measurement of Carbon-fiber/Epoxy Composite Materials (University of Nebraska) pg 108</t>
   </si>
   <si>
     <t>PTFE (General)</t>
@@ -323,6 +314,15 @@
   </si>
   <si>
     <t>http://www.toraycfa.com/product.html</t>
+  </si>
+  <si>
+    <t>http://www.matweb.com/search/MaterialGroupSearch.aspx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matweb </t>
+  </si>
+  <si>
+    <t>http://www.performancecomposites.com/about-composites-technical-info/124-designing-with-carbon-fiber.html</t>
   </si>
 </sst>
 </file>
@@ -402,10 +402,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -441,7 +441,7 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>72174</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>228069</xdr:rowOff>
+      <xdr:rowOff>189969</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -466,50 +466,6 @@
         <a:xfrm>
           <a:off x="7207250" y="4626059"/>
           <a:ext cx="2986824" cy="1863110"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>54272</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>8345</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>66899</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38A589BA-CCAD-473A-A96B-4F3F90A03E09}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6953250" y="4473872"/>
-          <a:ext cx="4580345" cy="2038277"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -820,61 +776,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>3</v>
       </c>
@@ -883,7 +839,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>4</v>
       </c>
@@ -892,7 +848,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>5</v>
       </c>
@@ -901,13 +857,13 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>63</v>
       </c>
@@ -916,125 +872,128 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>72</v>
       </c>
       <c r="D13" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="E13" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>74</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>76</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D16" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>47</v>
       </c>
       <c r="D18" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>69</v>
       </c>
       <c r="D19">
         <v>0.33</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>70</v>
       </c>
       <c r="D20" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
         <v>36</v>
       </c>
@@ -1045,21 +1004,24 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="I23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>37</v>
       </c>
@@ -1073,7 +1035,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>39</v>
       </c>
@@ -1087,7 +1049,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="3:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C26" s="4" t="s">
         <v>40</v>
       </c>
@@ -1101,7 +1063,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="4" t="s">
         <v>43</v>
       </c>
@@ -1115,7 +1077,7 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="4" t="s">
         <v>61</v>
       </c>
@@ -1129,7 +1091,7 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="3:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C29" s="5" t="s">
         <v>45</v>
       </c>
@@ -1143,7 +1105,7 @@
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="4" t="s">
         <v>37</v>
       </c>
@@ -1157,7 +1119,7 @@
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
         <v>47</v>
       </c>
@@ -1171,7 +1133,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C32" s="4" t="s">
         <v>49</v>
       </c>
@@ -1185,7 +1147,7 @@
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C33" s="4" t="s">
         <v>50</v>
       </c>
@@ -1198,11 +1160,8 @@
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
-      <c r="I33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C34" s="4" t="s">
         <v>52</v>
       </c>
@@ -1215,11 +1174,8 @@
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
-      <c r="I34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C35" s="4" t="s">
         <v>49</v>
       </c>
@@ -1232,11 +1188,8 @@
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
-      <c r="I35" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C36" s="4" t="s">
         <v>57</v>
       </c>
@@ -1250,7 +1203,7 @@
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C37" s="4" t="s">
         <v>59</v>
       </c>
@@ -1264,7 +1217,7 @@
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C38" s="4" t="s">
         <v>49</v>
       </c>
@@ -1278,7 +1231,7 @@
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="3:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C39" s="4" t="s">
         <v>54</v>
       </c>
@@ -1292,13 +1245,13 @@
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C41" s="2" t="s">
         <v>20</v>
       </c>
@@ -1307,7 +1260,7 @@
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>2</v>
       </c>
@@ -1321,97 +1274,97 @@
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C43" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D43" t="s">
         <v>23</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="8" t="s">
         <v>35</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C44" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D44" t="s">
         <v>25</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="8" t="s">
         <v>35</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C45" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D45" t="s">
         <v>28</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="8" t="s">
         <v>35</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C46" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D46" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="8" t="s">
         <v>35</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C47" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D47" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="8" t="s">
         <v>35</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C48" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D48" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E48" s="8" t="s">
         <v>35</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C50" s="2" t="s">
         <v>9</v>
       </c>
@@ -1420,7 +1373,7 @@
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>10</v>
       </c>
@@ -1434,7 +1387,7 @@
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>11</v>
       </c>
@@ -1448,7 +1401,7 @@
       <c r="G52" s="10"/>
       <c r="H52" s="10"/>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
         <v>15</v>
       </c>
@@ -1462,7 +1415,7 @@
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
     </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>17</v>
       </c>
@@ -1478,6 +1431,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="E41:H41"/>
+    <mergeCell ref="E43:H43"/>
+    <mergeCell ref="E44:H44"/>
+    <mergeCell ref="E45:H45"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="E46:H46"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="E54:H54"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="E50:H50"/>
+    <mergeCell ref="E51:H51"/>
+    <mergeCell ref="E52:H52"/>
+    <mergeCell ref="E53:H53"/>
     <mergeCell ref="E37:H37"/>
     <mergeCell ref="E38:H38"/>
     <mergeCell ref="E39:H39"/>
@@ -1494,37 +1478,6 @@
     <mergeCell ref="E29:H29"/>
     <mergeCell ref="E30:H30"/>
     <mergeCell ref="E31:H31"/>
-    <mergeCell ref="E46:H46"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="E54:H54"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="E50:H50"/>
-    <mergeCell ref="E51:H51"/>
-    <mergeCell ref="E52:H52"/>
-    <mergeCell ref="E53:H53"/>
-    <mergeCell ref="E41:H41"/>
-    <mergeCell ref="E43:H43"/>
-    <mergeCell ref="E44:H44"/>
-    <mergeCell ref="E45:H45"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="E32:H32"/>
-    <mergeCell ref="E33:H33"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E18:H18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1"/>

</xml_diff>